<commit_message>
updates to excel from the joint meeting
</commit_message>
<xml_diff>
--- a/אפיון בסיסי.xlsx
+++ b/אפיון בסיסי.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i022021/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i022021/dev/alonandella/dolibarr-extension/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4429FA51-BC90-8E41-BA47-B9BDCD9606D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA1F954-FA9E-5741-85DD-A18B601452C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13200" activeTab="1" xr2:uid="{B90DAB63-B41F-469C-9922-496D8A732978}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{B90DAB63-B41F-469C-9922-496D8A732978}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
   <si>
     <t>תהליך עבודה שוטף:</t>
   </si>
@@ -210,7 +210,63 @@
     <t xml:space="preserve">מעקב אחרי פעילות העובדים לצורך תיעוד המשימות שבוצעו ומעקב אחר יעילות העובדים. </t>
   </si>
   <si>
-    <t>0556621005</t>
+    <t>זמין כעת</t>
+  </si>
+  <si>
+    <t>מתוכנן</t>
+  </si>
+  <si>
+    <t>הערות</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>ממשק מהאתר - מתי שמוכנים</t>
+  </si>
+  <si>
+    <t>חסר ספקים לפעילות</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>"1/2"</t>
+  </si>
+  <si>
+    <t>לא אוטומטי</t>
+  </si>
+  <si>
+    <t>ללא חיבור אוטומטי. יצוא אקסל מותאם קיים דוגמא</t>
+  </si>
+  <si>
+    <t>אין מוצר לספק - רשימת מוצרים לרכישה אפשרי</t>
+  </si>
+  <si>
+    <t>כדי לא לחשוף מידע, צריך לדאוג לקרוא לפעילות בשם כללי, ורק בתיאור הפנימי להכניס פרטים רגישים</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>מחלקות בתוך הארגון?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">תבנית משימות לשירות? או תבנית של מספר משימות
+מלווה פרוייקט כתפקיד שאנשי קשר
+</t>
+  </si>
+  <si>
+    <t>הרשאות של משתמש שאינו מנהל - משמות שלו בלבד וכו׳</t>
+  </si>
+  <si>
+    <t>כרטסת לדוגמא ?</t>
+  </si>
+  <si>
+    <t>ארגון אב?</t>
+  </si>
+  <si>
+    <t>נושאים נוספים:</t>
   </si>
 </sst>
 </file>
@@ -254,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -262,6 +318,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,10 +717,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3E95E4-5E3E-4EE7-B111-B2CC561FE3B1}">
-  <dimension ref="A4:G22"/>
+  <dimension ref="A4:I26"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -668,9 +728,10 @@
     <col min="1" max="2" width="32.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -683,8 +744,17 @@
       <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -697,8 +767,14 @@
       <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="G5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
@@ -712,10 +788,13 @@
         <v>49</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="I6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -728,8 +807,14 @@
       <c r="D7" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="G7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -739,8 +824,14 @@
       <c r="C8" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="G8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -753,8 +844,14 @@
       <c r="D9" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="G9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -764,24 +861,39 @@
       <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="G10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="G11" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="G12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -791,13 +903,22 @@
       <c r="C13" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="G13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="G14" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
@@ -807,8 +928,14 @@
       <c r="C15" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="G15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
@@ -818,26 +945,54 @@
       <c r="C16" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>33</v>
+      </c>
+      <c r="G22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docu of change to system and excel changes
</commit_message>
<xml_diff>
--- a/אפיון בסיסי.xlsx
+++ b/אפיון בסיסי.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i022021/dev/alonandella/dolibarr-extension/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA1F954-FA9E-5741-85DD-A18B601452C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633EC6F8-83F8-6E46-B950-FEE33B3D8648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{B90DAB63-B41F-469C-9922-496D8A732978}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="2" xr2:uid="{B90DAB63-B41F-469C-9922-496D8A732978}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="אפיון " sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="90">
   <si>
     <t>תהליך עבודה שוטף:</t>
   </si>
@@ -267,6 +268,48 @@
   </si>
   <si>
     <t>נושאים נוספים:</t>
+  </si>
+  <si>
+    <t>דברים שחקרנו/פתרנו</t>
+  </si>
+  <si>
+    <t>פרוייקט אב</t>
+  </si>
+  <si>
+    <t>הערות על משימות ופרוייקטים</t>
+  </si>
+  <si>
+    <t>חברת אם</t>
+  </si>
+  <si>
+    <t>יבוא משימות</t>
+  </si>
+  <si>
+    <t>דף רישום</t>
+  </si>
+  <si>
+    <t>טיוטות של פרוייקטים</t>
+  </si>
+  <si>
+    <t>התממשקות עם מערכת פיננסית</t>
+  </si>
+  <si>
+    <t>דברים שאנחנו מצפים מאלון ואלה</t>
+  </si>
+  <si>
+    <t>ספקים לפעילות - כרגע לא מצאנו דרך מובנית - נדרש אפיון של מה התוצאה הנדרשת</t>
+  </si>
+  <si>
+    <t>איזה תהליכים מול המערכת הפיננסית רוצים לממשק? אפיון</t>
+  </si>
+  <si>
+    <t>פידבק כללי - והחלטה כללית אם התכולה הקיימת מספיקה להתחיל הטמעה - ואם לא, אז מה חסר</t>
+  </si>
+  <si>
+    <t>נדרש איפיון+תכנון של יבוא הנתונים מתוך האקסלים.</t>
+  </si>
+  <si>
+    <t>pdf font/alignment</t>
   </si>
 </sst>
 </file>
@@ -310,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -322,6 +365,9 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3E95E4-5E3E-4EE7-B111-B2CC561FE3B1}">
   <dimension ref="A4:I26"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView rightToLeft="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -999,4 +1045,92 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C01F3A-C9C3-C643-8AB9-36D2301B29A8}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="68" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>